<commit_message>
Completed Viewing,Scale,Translation Matric and Images
Signed-off-by: HydenJohnson75 <78604065+ToxicOddesey@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ImagesAndExcel/Assignment 1_HydenJohnson.xlsx
+++ b/ImagesAndExcel/Assignment 1_HydenJohnson.xlsx
@@ -1,25 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00220182\Desktop\CompG\ImagesAndExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITTralee Files YEAR 3\Computer Graphics\Repos\CompGraphics\ImagesAndExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDC03979-B774-4CEA-8A58-773D4C8BC4D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69185A87-3F7E-4E13-A28A-C8680AE73F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22635" yWindow="5805" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment generation" sheetId="1" r:id="rId1"/>
     <sheet name="Map of Assignment" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -390,7 +400,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -496,44 +506,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -565,10 +578,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>608240</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2365083</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>5089072</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -599,7 +612,556 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="3061607" y="326571"/>
-          <a:ext cx="1374322" cy="6132740"/>
+          <a:ext cx="1140440" cy="5089072"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>54429</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>204108</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1177269</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1347107</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393C3DCC-B487-908E-2A91-E11F5082D770}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1891393" y="6055179"/>
+          <a:ext cx="3626555" cy="1142999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>598714</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>137978</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>5089072</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5FD758A-4241-E97A-68DA-D875A5488DD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2435678" y="7973786"/>
+          <a:ext cx="2042979" cy="5143500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>40820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1199669</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1142999</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{138F1D19-8779-C43D-EC26-B2373AF594AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2000250" y="13593534"/>
+          <a:ext cx="3540098" cy="1102179"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>789215</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>391989</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>5170714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09D3E391-C90B-A088-BF5C-7A0AAD24C485}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2626179" y="15076714"/>
+          <a:ext cx="2106489" cy="5157107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>81643</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>136073</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1251857</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1152343</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A8F4B81-DCF7-6521-9CB3-71CD8FE2BACD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1918607" y="20723680"/>
+          <a:ext cx="3673929" cy="1016270"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>748393</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>575093</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>5116286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E848CBF-0B28-FA15-C8B8-9C544C916383}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2585357" y="22302108"/>
+          <a:ext cx="2330415" cy="5089071"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>176893</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>786493</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>934811</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E221EC6-54C9-F9AA-2924-15961A8F44DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7796893" y="13716000"/>
+          <a:ext cx="2446564" cy="771525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>37922</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>353786</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1264104</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1193346</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A03CD1B-3AAC-74AF-528F-74DA5162FA20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1874886" y="28153179"/>
+          <a:ext cx="3729897" cy="839560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>898072</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>373131</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>5116287</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18D704F1-6C27-C463-CB1A-C96FACE1DE00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2735036" y="29649964"/>
+          <a:ext cx="1978774" cy="5034644"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -619,19 +1181,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -958,7 +1507,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E13" sqref="C13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -972,24 +1521,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="K2" s="28" t="s">
         <v>36</v>
       </c>
@@ -1185,7 +1734,7 @@
   <dimension ref="A1:M91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E3"/>
+      <selection activeCell="D27" sqref="D27:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1209,10 +1758,10 @@
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="38"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="8"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1223,8 +1772,8 @@
     </row>
     <row r="3" spans="3:13" ht="408.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="5"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="47"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
       <c r="F3" s="33"/>
       <c r="G3" s="11"/>
       <c r="H3" s="34"/>
@@ -1244,20 +1793,20 @@
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="8"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
       <c r="L5" s="15"/>
       <c r="M5" s="12"/>
     </row>
-    <row r="6" spans="3:13" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:13" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="47"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="16"/>
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
@@ -1268,7 +1817,7 @@
     <row r="7" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="13"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
+      <c r="F7" s="35"/>
       <c r="G7" s="12"/>
       <c r="H7" s="15"/>
       <c r="I7" s="12"/>
@@ -1277,10 +1826,10 @@
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="38"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
       <c r="H8" s="15"/>
@@ -1288,10 +1837,10 @@
       <c r="L8" s="15"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="3:13" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="47"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="17"/>
       <c r="G9" s="12"/>
       <c r="H9" s="15"/>
@@ -1311,28 +1860,28 @@
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="5"/>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="41"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="45" t="s">
+      <c r="H11" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="46"/>
+      <c r="I11" s="43"/>
       <c r="J11" s="8"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="3:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:13" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="47"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="47"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="15"/>
@@ -1352,10 +1901,10 @@
     </row>
     <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="5"/>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="38"/>
+      <c r="E14" s="41"/>
       <c r="F14" s="17"/>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -1365,10 +1914,10 @@
       <c r="L14" s="15"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="3:13" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="5"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="47"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
       <c r="H15" s="15"/>
@@ -1392,10 +1941,10 @@
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="5"/>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="41"/>
       <c r="F17" s="18"/>
       <c r="G17" s="12"/>
       <c r="H17" s="15"/>
@@ -1405,10 +1954,10 @@
       <c r="L17" s="15"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="5"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="47"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
       <c r="F18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="12"/>
@@ -1429,31 +1978,31 @@
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="5"/>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="42" t="s">
+      <c r="E20" s="41"/>
+      <c r="F20" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="45" t="s">
+      <c r="G20" s="45"/>
+      <c r="H20" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="46"/>
+      <c r="I20" s="43"/>
       <c r="J20" s="17"/>
       <c r="K20" s="12"/>
       <c r="L20" s="15"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="5"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="47"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="39"/>
       <c r="J21" s="17"/>
       <c r="K21" s="12"/>
       <c r="L21" s="15"/>
@@ -1471,33 +2020,33 @@
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="5"/>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="38"/>
+      <c r="E23" s="41"/>
       <c r="F23" s="9"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="45" t="s">
+      <c r="L23" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="46"/>
+      <c r="M23" s="43"/>
     </row>
     <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="5"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="47"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
       <c r="F24" s="6"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="7"/>
       <c r="K24" s="23"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="47"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="39"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="13"/>
@@ -1510,22 +2059,22 @@
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="45" t="s">
+      <c r="D26" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="46"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="12"/>
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
       <c r="L26" s="15"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="47"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="39"/>
       <c r="F27" s="12"/>
       <c r="J27" s="15"/>
       <c r="K27" s="12"/>
@@ -1543,15 +2092,15 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="46"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="38"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="9"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -1562,11 +2111,11 @@
       <c r="M29" s="12"/>
     </row>
     <row r="30" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="41"/>
-      <c r="B30" s="47"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="47"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="39"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -1584,44 +2133,44 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="38"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="38"/>
-      <c r="F32" s="42" t="s">
+      <c r="E32" s="41"/>
+      <c r="F32" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="37" t="s">
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="38"/>
+      <c r="M32" s="41"/>
     </row>
     <row r="33" spans="1:13" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="39"/>
-      <c r="B33" s="40"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="46"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="44"/>
-      <c r="L33" s="41"/>
-      <c r="M33" s="40"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="46"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
@@ -1633,33 +2182,48 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C35" s="5"/>
-      <c r="D35" s="45" t="s">
+      <c r="D35" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="46"/>
+      <c r="E35" s="43"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C36" s="5"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="47"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="39"/>
       <c r="F36" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="40"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="46"/>
     </row>
     <row r="91" ht="0.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:G21"/>
@@ -1674,27 +2238,12 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Finsihed verticies and matricies
Signed-off-by: HydenJohnson75 <78604065+ToxicOddesey@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ImagesAndExcel/Assignment 1_HydenJohnson.xlsx
+++ b/ImagesAndExcel/Assignment 1_HydenJohnson.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00220182\Desktop\CompG\ImagesAndExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITTralee Files YEAR 3\Computer Graphics\Repos\CompGraphics\ImagesAndExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9F4F02-C0C2-4E0B-B27D-1FF5936AD22B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06970683-2EA5-4DD9-936D-62C923DB8255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22635" yWindow="5805" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15210" yWindow="3000" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment generation" sheetId="1" r:id="rId1"/>
     <sheet name="Map of Assignment" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -38,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>z = -1</t>
   </si>
@@ -164,6 +177,45 @@
   </si>
   <si>
     <t>Matrix.lookat();</t>
+  </si>
+  <si>
+    <t>0.1107863   ,   0.3066052</t>
+  </si>
+  <si>
+    <t>0.07753615   ,   0.5669309</t>
+  </si>
+  <si>
+    <t>0.2043844   ,   0.5404011</t>
+  </si>
+  <si>
+    <t>0.3802209   ,   0.3235788</t>
+  </si>
+  <si>
+    <t>0.5095453   ,   -0.0001543184</t>
+  </si>
+  <si>
+    <t>-1.235457   ,   -1.198137</t>
+  </si>
+  <si>
+    <t>0.3453664   ,   4.795619</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -0.07708043   ,   0.7698914</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -0.3834653   ,   1.0197</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -0.3124288   ,   1.078826</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -0.06615548   ,   0.8740009</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.05784526   ,   0.7210969</t>
+  </si>
+  <si>
+    <t>,-3.963956   ,   32.20899</t>
   </si>
 </sst>
 </file>
@@ -555,6 +607,1041 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Map of Assignment'!$G$45:$G$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>0.1107863</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7536149999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-7.7080430000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.38346530000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.31242880000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-6.6155480000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.7845260000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20438439999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.38022089999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.50954529999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.235457</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-3.963956</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.34536640000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2.517258</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.436342</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.350835</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-9.425741E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-7.9281240000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.19026560000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.43531170000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.3686912</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.16364119999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-6.9278279999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.8819609999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.1638867</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.20738219999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.86550680000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.3149093</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-2.1753300000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-1.6628039999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-1.141032</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.99072649999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Map of Assignment'!$H$45:$H$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>0.30660520000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56693090000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7698914</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0197000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0788260000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.87400089999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.72109690000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.54040109999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3235788</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.543184E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.198137</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32.20899</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.7956190000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6523559999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2614540000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.21452769999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-9.2124250000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.18962599999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.37918089999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.56215170000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.68392160000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.52593900000000005</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.37781350000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.2081277</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.180468E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.29997889999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-1.1553249999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-4.2432920000000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-10.56283</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.39582240000000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.38992569999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.45304309999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B5BE-4954-9E91-F247DAF3228D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="990817984"/>
+        <c:axId val="990818312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="990817984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="990818312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="990818312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="990817984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -743,67 +1830,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>898072</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>81643</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>373131</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>5116287</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18D704F1-6C27-C463-CB1A-C96FACE1DE00}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2735036" y="29649964"/>
-          <a:ext cx="1978774" cy="5034644"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>149679</xdr:rowOff>
@@ -828,7 +1854,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -844,67 +1870,6 @@
         <a:xfrm>
           <a:off x="2122714" y="13702393"/>
           <a:ext cx="3084740" cy="771525"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1496786</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>68036</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2245179</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>5171439</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{849A7C72-7D67-4DB8-993C-2F329B84E22B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3333750" y="15131143"/>
-          <a:ext cx="748393" cy="5103403"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -950,7 +1915,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -966,67 +1931,6 @@
         <a:xfrm>
           <a:off x="2203590" y="20778108"/>
           <a:ext cx="3090949" cy="907596"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1646465</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2318713</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>5143500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F3281AF-D5E4-4E59-8EC5-FCE24E62856B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3483429" y="22288500"/>
-          <a:ext cx="672248" cy="5129893"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1072,7 +1976,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1133,7 +2037,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1194,7 +2098,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1226,6 +2130,530 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>963707</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>515095</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>5143501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5C9B645-6F80-51A1-838E-5A735003734B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2779060" y="22176441"/>
+          <a:ext cx="2061506" cy="5132295"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>851648</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>380530</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>5132294</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CB5E320-CDCA-924F-EA02-91E88D2FE7A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2667001" y="15027088"/>
+          <a:ext cx="2039000" cy="5076265"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>773207</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>311091</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>5109883</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54BDD402-6F07-77DA-C3B6-0DF427176066}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2588560" y="29437853"/>
+          <a:ext cx="2048002" cy="5098677"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>705971</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>22411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>643778</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>793936</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C0EA66C-7097-ED1F-A25B-2D3A162EE929}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2521324" y="34962352"/>
+          <a:ext cx="2447925" cy="771525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>818030</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>358588</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>5131911</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F682B83-26BF-DD31-CA2B-2136BB8BF99E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2633383" y="36172589"/>
+          <a:ext cx="2050676" cy="5098293"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>907678</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>56030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>67237</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>5126463</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D9842F7-2106-7C5E-77EF-30C80267A79B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12091149" y="36195001"/>
+          <a:ext cx="2039470" cy="5070433"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>78440</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>294017</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>957542</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1141318</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24AAF487-2B92-84EF-1224-5C5275C2825B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11261911" y="27972546"/>
+          <a:ext cx="3759013" cy="847301"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>33130</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>16566</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>601146</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>4033631</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C533F862-2F4B-00AA-ECD7-AD3C710D001E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="33130" y="35151392"/>
+          <a:ext cx="1180929" cy="4017065"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>186359</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>115127</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>989772</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>42240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="26" name="Chart 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25C9A107-8542-1004-B568-610D527F7672}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1781,8 +3209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1791,7 +3219,7 @@
     <col min="4" max="4" width="37.5703125" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
     <col min="8" max="8" width="27.5703125" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="9.140625" customWidth="1"/>
@@ -2158,7 +3586,7 @@
       <c r="L29" s="15"/>
       <c r="M29" s="12"/>
     </row>
-    <row r="30" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="322.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="42"/>
       <c r="B30" s="43"/>
       <c r="C30" s="25"/>
@@ -2205,7 +3633,7 @@
       </c>
       <c r="M32" s="39"/>
     </row>
-    <row r="33" spans="1:13" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="40"/>
       <c r="B33" s="41"/>
       <c r="C33" s="17"/>
@@ -2248,9 +3676,314 @@
       <c r="H38" s="42"/>
       <c r="I38" s="41"/>
     </row>
+    <row r="45" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>42</v>
+      </c>
+      <c r="G45">
+        <v>0.1107863</v>
+      </c>
+      <c r="H45">
+        <v>0.30660520000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>43</v>
+      </c>
+      <c r="G46">
+        <v>7.7536149999999998E-2</v>
+      </c>
+      <c r="H46">
+        <v>0.56693090000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>49</v>
+      </c>
+      <c r="G47">
+        <v>-7.7080430000000005E-2</v>
+      </c>
+      <c r="H47">
+        <v>0.7698914</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E48" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48">
+        <v>-0.38346530000000001</v>
+      </c>
+      <c r="H48">
+        <v>1.0197000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>51</v>
+      </c>
+      <c r="G49">
+        <v>-0.31242880000000001</v>
+      </c>
+      <c r="H49">
+        <v>1.0788260000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>52</v>
+      </c>
+      <c r="G50">
+        <v>-6.6155480000000003E-2</v>
+      </c>
+      <c r="H50">
+        <v>0.87400089999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>53</v>
+      </c>
+      <c r="G51">
+        <v>5.7845260000000003E-2</v>
+      </c>
+      <c r="H51">
+        <v>0.72109690000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>44</v>
+      </c>
+      <c r="G52">
+        <v>0.20438439999999999</v>
+      </c>
+      <c r="H52">
+        <v>0.54040109999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>45</v>
+      </c>
+      <c r="G53">
+        <v>0.38022089999999997</v>
+      </c>
+      <c r="H53">
+        <v>0.3235788</v>
+      </c>
+    </row>
+    <row r="54" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>46</v>
+      </c>
+      <c r="G54">
+        <v>0.50954529999999998</v>
+      </c>
+      <c r="H54">
+        <v>-1.543184E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>47</v>
+      </c>
+      <c r="G55">
+        <v>-1.235457</v>
+      </c>
+      <c r="H55">
+        <v>-1.198137</v>
+      </c>
+    </row>
+    <row r="56" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E56" t="s">
+        <v>54</v>
+      </c>
+      <c r="G56">
+        <v>-3.963956</v>
+      </c>
+      <c r="H56">
+        <v>32.20899</v>
+      </c>
+    </row>
+    <row r="57" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
+        <v>48</v>
+      </c>
+      <c r="G57">
+        <v>0.34536640000000002</v>
+      </c>
+      <c r="H57">
+        <v>4.7956190000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>-2.517258</v>
+      </c>
+      <c r="H58">
+        <v>1.6523559999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>-1.436342</v>
+      </c>
+      <c r="H59">
+        <v>1.2614540000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>-1.350835</v>
+      </c>
+      <c r="H60">
+        <v>0.21452769999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G61">
+        <v>-9.425741E-2</v>
+      </c>
+      <c r="H61">
+        <v>-9.2124250000000005E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <v>-7.9281240000000003E-2</v>
+      </c>
+      <c r="H62">
+        <v>0.18962599999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G63">
+        <v>-0.19026560000000001</v>
+      </c>
+      <c r="H63">
+        <v>0.37918089999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G64">
+        <v>-0.43531170000000002</v>
+      </c>
+      <c r="H64">
+        <v>0.56215170000000003</v>
+      </c>
+    </row>
+    <row r="65" spans="7:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>-0.3686912</v>
+      </c>
+      <c r="H65">
+        <v>0.68392160000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="7:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G66">
+        <v>-0.16364119999999999</v>
+      </c>
+      <c r="H66">
+        <v>0.52593900000000005</v>
+      </c>
+    </row>
+    <row r="67" spans="7:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G67">
+        <v>-6.9278279999999998E-2</v>
+      </c>
+      <c r="H67">
+        <v>0.37781350000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="7:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G68">
+        <v>3.8819609999999997E-2</v>
+      </c>
+      <c r="H68">
+        <v>0.2081277</v>
+      </c>
+    </row>
+    <row r="69" spans="7:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G69">
+        <v>0.1638867</v>
+      </c>
+      <c r="H69">
+        <v>1.180468E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="7:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G70">
+        <v>0.20738219999999999</v>
+      </c>
+      <c r="H70">
+        <v>-0.29997889999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="7:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G71">
+        <v>-0.86550680000000002</v>
+      </c>
+      <c r="H71">
+        <v>-1.1553249999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="7:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G72">
+        <v>-0.3149093</v>
+      </c>
+      <c r="H72">
+        <v>-4.2432920000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="7:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G73">
+        <v>-2.1753300000000002</v>
+      </c>
+      <c r="H73">
+        <v>-10.56283</v>
+      </c>
+    </row>
+    <row r="74" spans="7:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G74">
+        <v>-1.6628039999999999</v>
+      </c>
+      <c r="H74">
+        <v>0.39582240000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="7:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G75">
+        <v>-1.141032</v>
+      </c>
+      <c r="H75">
+        <v>0.38992569999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="7:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G76">
+        <v>-0.99072649999999995</v>
+      </c>
+      <c r="H76">
+        <v>-0.45304309999999998</v>
+      </c>
+    </row>
     <row r="91" ht="0.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D18:E18"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E3"/>
@@ -2258,19 +3991,9 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
     <mergeCell ref="H21:I21"/>
-    <mergeCell ref="D11:E11"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H12:I12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="D30:E30"/>

</xml_diff>